<commit_message>
Updated excel with results
</commit_message>
<xml_diff>
--- a/tests_results.xlsx
+++ b/tests_results.xlsx
@@ -18,53 +18,84 @@
   <commentList>
     <comment authorId="0" ref="B3">
       <text>
-        <t xml:space="preserve">AL IMPORTAR: Parece que no encuentra el nodo de entrada de la capa densa de salida al empezar a recorrer el grafo (desde la salida)
+        <t xml:space="preserve">IN IMPORT: Raises an error when looking for the nodes inputs. Is not able to find the input of a dense node (seems to be the first processed layer).
 </t>
       </text>
     </comment>
     <comment authorId="0" ref="C3">
       <text>
-        <t xml:space="preserve">AL IMPORTAR: EL ONNX checker da error porque detecta un nodo que no es output de otro. Porque requiere que los nodos estén ordenados topológicamente y al parecer no lo están </t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="G3">
-      <text>
-        <t xml:space="preserve">Al EXPORTAR: Error del parser de tf con el nombre de un operador (parece que es el maxPool1D por el orden de los logs)</t>
+        <t xml:space="preserve">IN IMPORT: The ONNX checker raises an error due to the order of the nodes that is not in topological order. Although with ONNX RT it does work </t>
       </text>
     </comment>
     <comment authorId="0" ref="H3">
       <text>
-        <t xml:space="preserve">AL EXPORTAR: Ver nota de TF/Keras</t>
+        <t xml:space="preserve">IN EXPORT: Raises an error when parsing the operators names</t>
       </text>
     </comment>
     <comment authorId="0" ref="I3">
       <text>
-        <t xml:space="preserve">AL EXPORTAR: Ver nota de TF/Keras</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="L3">
-      <text>
-        <t xml:space="preserve">AL IMPORTAR: No encuentra el input de una capa. Al usar el onnx checker da error porque el orden de los nodos parece no estar en orden topológico ( podría no funcionar por esto)</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="M3">
-      <text>
-        <t xml:space="preserve">AL IMPORTAR: Fallael onnx checker por el orden de los nodos, que tiene que ser en orden topológico</t>
+        <t xml:space="preserve">IN EXPORT: Raises an error when parsing the operators names</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="J3">
+      <text>
+        <t xml:space="preserve">IN EXPORT: Raises an error when parsing the operators names</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="K3">
+      <text>
+        <t xml:space="preserve">IN EXPORT: Raises an error when parsing the operators names</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="N3">
+      <text>
+        <t xml:space="preserve">IN IMPORT: The ONNX checker raises an error beacuse the nodes are not topologically sorted and in the transformation to the keras model it raises an error beacuse of an input of a node is not found</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="O3">
+      <text>
+        <t xml:space="preserve">IN IMPORT: The ONNX checker raises an error beacuse the nodes are not topologically sorted. And this check is inside the pytorch function.</t>
       </text>
     </comment>
     <comment authorId="0" ref="B4">
       <text>
-        <t xml:space="preserve">AL IMPORTAR: mismo error que al exportar desde tf </t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="G4">
-      <text>
-        <t xml:space="preserve">AL IMPORTAR: mismo error que en conv2D</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="L4">
-      <text>
-        <t xml:space="preserve">Al IMPORTAR: El onnx checker da el OK pero la transformación al modelo de keras falla porque dice que no encuentra un input. Mismo error que de keras -&gt; keras pero esta vez el onnx checker da OK</t>
+        <t xml:space="preserve">In IMPORT: Same error than the keras to keras import.</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="H4">
+      <text>
+        <t xml:space="preserve">IN IMPORT: Raises an error when looking for the nodes inputs. Is not able to find the input of a dense node (seems to be the first processed layer).
+</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="N4">
+      <text>
+        <t xml:space="preserve">IN IMPORT: The ONNX checker gives an OK but in the transformation to the keras model it raises an error beacuse of an input of a node is not found</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="B5">
+      <text>
+        <t xml:space="preserve">In IMPORT: Same error than the keras to keras import.</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="C5">
+      <text>
+        <t xml:space="preserve">IN IMPORT: It can't find the weights initializers. Says "IndexError: Input conv1_W is undefined!" but conv1_W is in the initializers section (checked with the onnx library)</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="H5">
+      <text>
+        <t xml:space="preserve">In IMPORT: Raises the error "TypeError: 'Lambda' object does not support item assignment". </t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="I5">
+      <text>
+        <t xml:space="preserve">IN IMPORT: It can't find the weights initializers. Says "IndexError: Input conv1D1_W is undefined!" but conv1D1_W is in the initializers section (checked with the onnx library)</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="Q5">
+      <text>
+        <t xml:space="preserve">IMPORT: EDDL uses 2D inputs for LSTM, and ONNX RT needs 3D tensors (with seq_length)</t>
       </text>
     </comment>
   </commentList>
@@ -72,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="13">
   <si>
     <t>MNIST 2D Conv</t>
   </si>
@@ -92,10 +123,16 @@
     <t>Pytorch</t>
   </si>
   <si>
+    <t>EDDL</t>
+  </si>
+  <si>
     <t>ONNX RT</t>
   </si>
   <si>
     <t>FAIL</t>
+  </si>
+  <si>
+    <t>GOAL</t>
   </si>
   <si>
     <t>OK</t>
@@ -108,7 +145,7 @@
       <t>TF/Keras:</t>
     </r>
     <r>
-      <t xml:space="preserve"> Hay que utilizar librerías externas, una para importar (onnx2keras) y otra para exportar (keras2onnx). Además, la carga del archivo ONNX se hace con la librería onnx de python.</t>
+      <t xml:space="preserve"> You need external libraries, for importing (onnx2keras, from unknown third party repo) and for exporting (keras2onnx, from onnx repo). They use the onnx python library to read the onnx file before doing the conversion to TF/Keras. The exporting seems to be good because it is done by the onnx team (but fails for the 1D Conv case). The importing doesn't work in any case, it has problems with finding the nodes input connections.</t>
     </r>
   </si>
   <si>
@@ -119,7 +156,7 @@
       <t>Pytorch:</t>
     </r>
     <r>
-      <t xml:space="preserve"> Utilizan la librería onnx de python para cargar el onnx. Y la importación no está incluida directamente en "torch", sino que está dentro de la librería caffe2</t>
+      <t xml:space="preserve"> They use the onnx python library to load the onnx file, and then, they make the transformation to the pytorch model. This transformation is not made by the "torch" library, instead of that, it is in the caffe2 library wich is of facebook too. When exporting, to make it work it is necessary to activate the flag "keep_initializers_as_inputs" in the export function.</t>
     </r>
   </si>
 </sst>
@@ -143,6 +180,8 @@
     <font>
       <b/>
       <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
     <font>
       <sz val="11.0"/>
@@ -150,8 +189,6 @@
       <name val="Arial"/>
     </font>
     <font>
-      <b/>
-      <sz val="11.0"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
@@ -214,7 +251,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -233,20 +270,17 @@
     <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
     <dxf>
       <font/>
       <fill>
@@ -263,6 +297,16 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFFF0000"/>
           <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
       <border/>
@@ -480,8 +524,8 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="16.43"/>
-    <col customWidth="1" min="6" max="6" width="17.57"/>
-    <col customWidth="1" min="11" max="11" width="18.14"/>
+    <col customWidth="1" min="7" max="7" width="17.57"/>
+    <col customWidth="1" min="13" max="13" width="18.14"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -490,19 +534,22 @@
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
-      <c r="D1" s="3"/>
-      <c r="F1" s="1" t="s">
+      <c r="D1" s="2"/>
+      <c r="E1" s="3"/>
+      <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="2"/>
       <c r="H1" s="2"/>
-      <c r="I1" s="3"/>
-      <c r="K1" s="1" t="s">
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="3"/>
+      <c r="M1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="3"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="3"/>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
@@ -517,31 +564,40 @@
       <c r="D2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="4" t="s">
+      <c r="E2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="G2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="6"/>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2" s="6"/>
+      <c r="M2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="N2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="O2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="P2" s="5" t="s">
         <v>6</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3">
@@ -549,39 +605,48 @@
         <v>4</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="7" t="s">
-        <v>7</v>
-      </c>
       <c r="H3" s="7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3" s="6"/>
-      <c r="K3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" s="6"/>
+      <c r="M3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>7</v>
-      </c>
       <c r="N3" s="7" t="s">
         <v>8</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="P3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q3" s="7" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4">
@@ -589,83 +654,133 @@
         <v>5</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="6"/>
+      <c r="G4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="7" t="s">
-        <v>7</v>
-      </c>
       <c r="H4" s="7" t="s">
         <v>8</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="J4" s="6"/>
-      <c r="K4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" s="6"/>
+      <c r="M4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>8</v>
-      </c>
       <c r="N4" s="7" t="s">
         <v>8</v>
+      </c>
+      <c r="O4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q4" s="7" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="8"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
+      <c r="A5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5" s="6"/>
+      <c r="M5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="O5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q5" s="5" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" s="10" t="s">
-        <v>9</v>
-      </c>
+      <c r="A7" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" ht="29.25" customHeight="1">
+      <c r="G11" s="9"/>
     </row>
     <row r="14">
-      <c r="A14" s="10" t="s">
-        <v>10</v>
+      <c r="A14" s="8" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="A7:D11"/>
-    <mergeCell ref="A14:D18"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="M1:Q1"/>
+    <mergeCell ref="A7:E11"/>
+    <mergeCell ref="A14:E18"/>
   </mergeCells>
-  <conditionalFormatting sqref="B3:D5 G3:I5 L3:N5">
+  <conditionalFormatting sqref="B3:E5 H3:K5 N3:Q5">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH(("OK"),(B3))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3:D5 G3:I5 L3:N5">
+  <conditionalFormatting sqref="B3:E5 H3:K5 N3:Q5">
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH(("FAIL"),(B3))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3:E5 H3:K5 N3:Q5">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="GOAL">
+      <formula>NOT(ISERROR(SEARCH(("GOAL"),(B3))))</formula>
     </cfRule>
   </conditionalFormatting>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
Added lstm enc dec mnist import and updated the spreadsheet
</commit_message>
<xml_diff>
--- a/tests_results.xlsx
+++ b/tests_results.xlsx
@@ -57,6 +57,21 @@
         <t xml:space="preserve">IN IMPORT: The ONNX checker raises an error beacuse the nodes are not topologically sorted. And this check is inside the pytorch function.</t>
       </text>
     </comment>
+    <comment authorId="0" ref="T3">
+      <text>
+        <t xml:space="preserve">IN IMPORT: It can't find the input of a node.</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="U3">
+      <text>
+        <t xml:space="preserve">IN IMPORT: Raises an error because the nodes are not topologically sorted in the onnx object.</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="W3">
+      <text>
+        <t xml:space="preserve">The loss value is not the same. From 0.01158 to 0.10749</t>
+      </text>
+    </comment>
     <comment authorId="0" ref="B4">
       <text>
         <t xml:space="preserve">In IMPORT: Same error than the keras to keras import.</t>
@@ -73,6 +88,21 @@
         <t xml:space="preserve">IN IMPORT: The ONNX checker gives an OK but in the transformation to the keras model it raises an error beacuse of an input of a node is not found</t>
       </text>
     </comment>
+    <comment authorId="0" ref="P4">
+      <text>
+        <t xml:space="preserve">TODO: Fix the  recurrent bias of the LSTM included in the ONNX created by Pytorch</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="T4">
+      <text>
+        <t xml:space="preserve">IN IMPORT: It can't find the input of a node.</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="U4">
+      <text>
+        <t xml:space="preserve">IN IMPORT: The loss value is not the same. From 0.0085 to 0.20495 (almost the same mse value than with an untrained net)</t>
+      </text>
+    </comment>
     <comment authorId="0" ref="B5">
       <text>
         <t xml:space="preserve">In IMPORT: Same error than the keras to keras import.</t>
@@ -93,9 +123,29 @@
         <t xml:space="preserve">IN IMPORT: It can't find the weights initializers. Says "IndexError: Input conv1D1_W is undefined!" but conv1D1_W is in the initializers section (checked with the onnx library)</t>
       </text>
     </comment>
+    <comment authorId="0" ref="N5">
+      <text>
+        <t xml:space="preserve">IN IMPORT: The ONNX checker gives an OK but in the transformation to the keras model it raises an error beacuse the input of the first node is not found</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="O5">
+      <text>
+        <t xml:space="preserve">IN IMPORT: It can't find the weights initializers. Says "IndexError: Input embedding1_data is undefined!" but embedding1_data is in the initializers section (checked with the onnx library)</t>
+      </text>
+    </comment>
     <comment authorId="0" ref="Q5">
       <text>
         <t xml:space="preserve">IMPORT: EDDL uses 2D inputs for LSTM, and ONNX RT needs 3D tensors (with seq_length)</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="T5">
+      <text>
+        <t xml:space="preserve">IN IMPORT: It can't find the input of a node.</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="U5">
+      <text>
+        <t xml:space="preserve">IN IMPORT: Raises an error because the nodes are not topologically sorted in the onnx object.</t>
       </text>
     </comment>
   </commentList>
@@ -103,7 +153,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="13">
   <si>
     <t>MNIST 2D Conv</t>
   </si>
@@ -114,6 +164,9 @@
     <t>IMDB LSTM</t>
   </si>
   <si>
+    <t>LSTM with Decoder</t>
+  </si>
+  <si>
     <t>Export \ Import</t>
   </si>
   <si>
@@ -130,9 +183,6 @@
   </si>
   <si>
     <t>FAIL</t>
-  </si>
-  <si>
-    <t>GOAL</t>
   </si>
   <si>
     <t>OK</t>
@@ -145,7 +195,16 @@
       <t>TF/Keras:</t>
     </r>
     <r>
-      <t xml:space="preserve"> You need external libraries, for importing (onnx2keras, from unknown third party repo) and for exporting (keras2onnx, from onnx repo). They use the onnx python library to read the onnx file before doing the conversion to TF/Keras. The exporting seems to be good because it is done by the onnx team (but fails for the 1D Conv case). The importing doesn't work in any case, it has problems with finding the nodes input connections.</t>
+      <t xml:space="preserve"> You need external libraries, for importing (onnx2keras, from unknown </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+      </rPr>
+      <t>third party repo</t>
+    </r>
+    <r>
+      <t>) and for exporting (keras2onnx, from onnx repo). They use the onnx python library to read the onnx file before doing the conversion to TF/Keras. The exporting seems to be good because it is done by the onnx team (but fails for the 1D Conv case). The importing doesn't work in any case, it has problems with finding the nodes input connections.</t>
     </r>
   </si>
   <si>
@@ -156,7 +215,7 @@
       <t>Pytorch:</t>
     </r>
     <r>
-      <t xml:space="preserve"> They use the onnx python library to load the onnx file, and then, they make the transformation to the pytorch model. This transformation is not made by the "torch" library, instead of that, it is in the caffe2 library wich is of facebook too. When exporting, to make it work it is necessary to activate the flag "keep_initializers_as_inputs" in the export function.</t>
+      <t xml:space="preserve"> They use the onnx python library to load the onnx file, and then, they make the transformation to the pytorch model. This transformation is not made by the "torch" library, instead of that, it is in the caffe2 library wich is of facebook too. When exporting, to make it work it is necessary to activate the flag "keep_initializers_as_inputs" in the export function. To import the ONNX models with the EDDL is convenient to use the onnx simplifier (https://github.com/daquexian/onnx-simplifier).</t>
     </r>
   </si>
 </sst>
@@ -526,6 +585,7 @@
     <col customWidth="1" min="1" max="1" width="16.43"/>
     <col customWidth="1" min="7" max="7" width="17.57"/>
     <col customWidth="1" min="13" max="13" width="18.14"/>
+    <col customWidth="1" min="19" max="19" width="18.0"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -550,111 +610,148 @@
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="3"/>
+      <c r="S1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="3"/>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L2" s="6"/>
       <c r="M2" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="S2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="T2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="U2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="V2" s="5" t="s">
         <v>7</v>
+      </c>
+      <c r="W2" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L3" s="6"/>
       <c r="M3" s="5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="N3" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="O3" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="P3" s="7" t="s">
         <v>10</v>
       </c>
       <c r="Q3" s="7" t="s">
         <v>10</v>
+      </c>
+      <c r="S3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="T3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="U3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="V3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="W3" s="7" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>10</v>
@@ -667,10 +764,10 @@
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I4" s="7" t="s">
         <v>10</v>
@@ -683,30 +780,45 @@
       </c>
       <c r="L4" s="6"/>
       <c r="M4" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N4" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="O4" s="7" t="s">
         <v>10</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="Q4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="S4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="T4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="U4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="V4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="W4" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>10</v>
@@ -716,13 +828,13 @@
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J5" s="5" t="s">
         <v>10</v>
@@ -732,7 +844,7 @@
       </c>
       <c r="L5" s="6"/>
       <c r="M5" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N5" s="7" t="s">
         <v>9</v>
@@ -744,6 +856,21 @@
         <v>10</v>
       </c>
       <c r="Q5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="S5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="T5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="U5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="V5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="W5" s="5" t="s">
         <v>10</v>
       </c>
     </row>
@@ -761,24 +888,25 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="G1:K1"/>
     <mergeCell ref="M1:Q1"/>
+    <mergeCell ref="S1:W1"/>
     <mergeCell ref="A7:E11"/>
-    <mergeCell ref="A14:E18"/>
+    <mergeCell ref="A14:E20"/>
   </mergeCells>
-  <conditionalFormatting sqref="B3:E5 H3:K5 N3:Q5">
+  <conditionalFormatting sqref="B3:E5 H3:K5 N3:Q5 T3:W5">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH(("OK"),(B3))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3:E5 H3:K5 N3:Q5">
+  <conditionalFormatting sqref="B3:E5 H3:K5 N3:Q5 T3:W5">
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH(("FAIL"),(B3))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3:E5 H3:K5 N3:Q5">
+  <conditionalFormatting sqref="B3:E5 H3:K5 N3:Q5 T3:W5">
     <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="GOAL">
       <formula>NOT(ISERROR(SEARCH(("GOAL"),(B3))))</formula>
     </cfRule>

</xml_diff>